<commit_message>
Fix circular reference in Cash Flow Statement
Fixed two critical issues in the Cash Flow Statement:

1. Circular reference in Operating Activities (line 1429):
   - Changed from: =SUM(B6:B16) which included row 16 in its own sum
   - Changed to: =B6+B8+SUM(B10:B15) which excludes the total row
   - This eliminates the circular reference while correctly summing:
     * Net Income (row 6)
     * Depreciation (row 8)
     * Working capital changes (rows 10-15)

2. Incorrect row references in Net Change calculation (line 1488):
   - Changed from: =B17+B21+B26 (blank rows)
   - Changed to: =B16+B20+B25 (actual subtotals)
   - Now correctly sums:
     * Cash from Operating Activities (row 16)
     * Cash from Investing Activities (row 20)
     * Cash from Financing Activities (row 25)

Model now calculates correctly without circular references.
</commit_message>
<xml_diff>
--- a/Financial_Model_3_Statement.xlsx
+++ b/Financial_Model_3_Statement.xlsx
@@ -6310,51 +6310,51 @@
         </is>
       </c>
       <c r="B16" s="13">
-        <f>SUM(B6:B16)</f>
+        <f>B6+B8+SUM(B10:B15)</f>
         <v/>
       </c>
       <c r="C16" s="13">
-        <f>SUM(C6:C16)</f>
+        <f>C6+C8+SUM(C10:C15)</f>
         <v/>
       </c>
       <c r="D16" s="13">
-        <f>SUM(D6:D16)</f>
+        <f>D6+D8+SUM(D10:D15)</f>
         <v/>
       </c>
       <c r="E16" s="13">
-        <f>SUM(E6:E16)</f>
+        <f>E6+E8+SUM(E10:E15)</f>
         <v/>
       </c>
       <c r="F16" s="13">
-        <f>SUM(F6:F16)</f>
+        <f>F6+F8+SUM(F10:F15)</f>
         <v/>
       </c>
       <c r="G16" s="13">
-        <f>SUM(G6:G16)</f>
+        <f>G6+G8+SUM(G10:G15)</f>
         <v/>
       </c>
       <c r="H16" s="13">
-        <f>SUM(H6:H16)</f>
+        <f>H6+H8+SUM(H10:H15)</f>
         <v/>
       </c>
       <c r="I16" s="13">
-        <f>SUM(I6:I16)</f>
+        <f>I6+I8+SUM(I10:I15)</f>
         <v/>
       </c>
       <c r="J16" s="13">
-        <f>SUM(J6:J16)</f>
+        <f>J6+J8+SUM(J10:J15)</f>
         <v/>
       </c>
       <c r="K16" s="13">
-        <f>SUM(K6:K16)</f>
+        <f>K6+K8+SUM(K10:K15)</f>
         <v/>
       </c>
       <c r="L16" s="13">
-        <f>SUM(L6:L16)</f>
+        <f>L6+L8+SUM(L10:L15)</f>
         <v/>
       </c>
       <c r="M16" s="13">
-        <f>SUM(M6:M16)</f>
+        <f>M6+M8+SUM(M10:M15)</f>
         <v/>
       </c>
     </row>
@@ -6642,51 +6642,51 @@
         </is>
       </c>
       <c r="B27" s="15">
-        <f>B17+B21+B26</f>
+        <f>B16+B20+B25</f>
         <v/>
       </c>
       <c r="C27" s="15">
-        <f>C17+C21+C26</f>
+        <f>C16+C20+C25</f>
         <v/>
       </c>
       <c r="D27" s="15">
-        <f>D17+D21+D26</f>
+        <f>D16+D20+D25</f>
         <v/>
       </c>
       <c r="E27" s="15">
-        <f>E17+E21+E26</f>
+        <f>E16+E20+E25</f>
         <v/>
       </c>
       <c r="F27" s="15">
-        <f>F17+F21+F26</f>
+        <f>F16+F20+F25</f>
         <v/>
       </c>
       <c r="G27" s="15">
-        <f>G17+G21+G26</f>
+        <f>G16+G20+G25</f>
         <v/>
       </c>
       <c r="H27" s="15">
-        <f>H17+H21+H26</f>
+        <f>H16+H20+H25</f>
         <v/>
       </c>
       <c r="I27" s="15">
-        <f>I17+I21+I26</f>
+        <f>I16+I20+I25</f>
         <v/>
       </c>
       <c r="J27" s="15">
-        <f>J17+J21+J26</f>
+        <f>J16+J20+J25</f>
         <v/>
       </c>
       <c r="K27" s="15">
-        <f>K17+K21+K26</f>
+        <f>K16+K20+K25</f>
         <v/>
       </c>
       <c r="L27" s="15">
-        <f>L17+L21+L26</f>
+        <f>L16+L20+L25</f>
         <v/>
       </c>
       <c r="M27" s="15">
-        <f>M17+M21+M26</f>
+        <f>M16+M20+M25</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix Net Income row references in formulas
Corrected Net Income row reference from row 20 to row 19:
- Income Statement Net Income is on row 19, not row 20
- Fixed Cash Flow Statement reference (line 1340)
- Fixed Retained Earnings control account reference (line 850)

Both now correctly reference 'Income Statement'!B19 instead of B20.

All formulas now properly integrated:
- Cash Flow Statement pulls correct Net Income
- Retained Earnings control adds correct Net Income
- Complete 3-statement integration verified
</commit_message>
<xml_diff>
--- a/Financial_Model_3_Statement.xlsx
+++ b/Financial_Model_3_Statement.xlsx
@@ -3439,51 +3439,51 @@
         </is>
       </c>
       <c r="B74" s="12">
-        <f>'Income Statement'!B20</f>
+        <f>'Income Statement'!B19</f>
         <v/>
       </c>
       <c r="C74" s="12">
-        <f>'Income Statement'!C20</f>
+        <f>'Income Statement'!C19</f>
         <v/>
       </c>
       <c r="D74" s="12">
-        <f>'Income Statement'!D20</f>
+        <f>'Income Statement'!D19</f>
         <v/>
       </c>
       <c r="E74" s="12">
-        <f>'Income Statement'!E20</f>
+        <f>'Income Statement'!E19</f>
         <v/>
       </c>
       <c r="F74" s="12">
-        <f>'Income Statement'!F20</f>
+        <f>'Income Statement'!F19</f>
         <v/>
       </c>
       <c r="G74" s="12">
-        <f>'Income Statement'!G20</f>
+        <f>'Income Statement'!G19</f>
         <v/>
       </c>
       <c r="H74" s="12">
-        <f>'Income Statement'!H20</f>
+        <f>'Income Statement'!H19</f>
         <v/>
       </c>
       <c r="I74" s="12">
-        <f>'Income Statement'!I20</f>
+        <f>'Income Statement'!I19</f>
         <v/>
       </c>
       <c r="J74" s="12">
-        <f>'Income Statement'!J20</f>
+        <f>'Income Statement'!J19</f>
         <v/>
       </c>
       <c r="K74" s="12">
-        <f>'Income Statement'!K20</f>
+        <f>'Income Statement'!K19</f>
         <v/>
       </c>
       <c r="L74" s="12">
-        <f>'Income Statement'!L20</f>
+        <f>'Income Statement'!L19</f>
         <v/>
       </c>
       <c r="M74" s="12">
-        <f>'Income Statement'!M20</f>
+        <f>'Income Statement'!M19</f>
         <v/>
       </c>
     </row>
@@ -5856,51 +5856,51 @@
         </is>
       </c>
       <c r="B6" s="12">
-        <f>'Income Statement'!B20</f>
+        <f>'Income Statement'!B19</f>
         <v/>
       </c>
       <c r="C6" s="12">
-        <f>'Income Statement'!C20</f>
+        <f>'Income Statement'!C19</f>
         <v/>
       </c>
       <c r="D6" s="12">
-        <f>'Income Statement'!D20</f>
+        <f>'Income Statement'!D19</f>
         <v/>
       </c>
       <c r="E6" s="12">
-        <f>'Income Statement'!E20</f>
+        <f>'Income Statement'!E19</f>
         <v/>
       </c>
       <c r="F6" s="12">
-        <f>'Income Statement'!F20</f>
+        <f>'Income Statement'!F19</f>
         <v/>
       </c>
       <c r="G6" s="12">
-        <f>'Income Statement'!G20</f>
+        <f>'Income Statement'!G19</f>
         <v/>
       </c>
       <c r="H6" s="12">
-        <f>'Income Statement'!H20</f>
+        <f>'Income Statement'!H19</f>
         <v/>
       </c>
       <c r="I6" s="12">
-        <f>'Income Statement'!I20</f>
+        <f>'Income Statement'!I19</f>
         <v/>
       </c>
       <c r="J6" s="12">
-        <f>'Income Statement'!J20</f>
+        <f>'Income Statement'!J19</f>
         <v/>
       </c>
       <c r="K6" s="12">
-        <f>'Income Statement'!K20</f>
+        <f>'Income Statement'!K19</f>
         <v/>
       </c>
       <c r="L6" s="12">
-        <f>'Income Statement'!L20</f>
+        <f>'Income Statement'!L19</f>
         <v/>
       </c>
       <c r="M6" s="12">
-        <f>'Income Statement'!M20</f>
+        <f>'Income Statement'!M19</f>
         <v/>
       </c>
     </row>

</xml_diff>